<commit_message>
generateReport: Move xlsx generation to frontend
</commit_message>
<xml_diff>
--- a/public/balances.xlsx
+++ b/public/balances.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Augusto Carosi" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Caja central" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Juan Pablo Carosi Warburg" state="visible" r:id="rId6"/>
-    <sheet sheetId="4" name="Martín della Paolera" state="visible" r:id="rId7"/>
-    <sheet sheetId="5" name="Alejandro Penovi" state="visible" r:id="rId8"/>
+    <sheet sheetId="2" name="Juan Pablo Carosi Warburg" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Alejandro Penovi" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="Caja central" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="Jorge Garcia" state="visible" r:id="rId8"/>
     <sheet sheetId="6" name="Fernando Bella" state="visible" r:id="rId9"/>
-    <sheet sheetId="7" name="Jorge Garcia" state="visible" r:id="rId10"/>
+    <sheet sheetId="7" name="Martín della Paolera" state="visible" r:id="rId10"/>
     <sheet sheetId="8" name="Lautaro Molina" state="visible" r:id="rId11"/>
     <sheet sheetId="9" name="Resumen de centros de costo" state="visible" r:id="rId12"/>
   </sheets>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -60,60 +60,120 @@
     <t>Reposicion de caja</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Un ticket</t>
+  </si>
+  <si>
+    <t>GSP, PICC</t>
+  </si>
+  <si>
+    <t>combustible</t>
+  </si>
+  <si>
+    <t>Una caja</t>
+  </si>
+  <si>
+    <t>Caja nuvea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combustible </t>
+  </si>
+  <si>
+    <t>LEON</t>
+  </si>
+  <si>
+    <t>Pintura</t>
+  </si>
+  <si>
+    <t>otros</t>
+  </si>
+  <si>
+    <t>Combustible leonardo</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Bandejas pintor</t>
+  </si>
+  <si>
+    <t>Combustible</t>
+  </si>
+  <si>
+    <t>Alquiler martillete</t>
+  </si>
+  <si>
+    <t>BOAT</t>
+  </si>
+  <si>
+    <t>Flete deculucion andamios</t>
+  </si>
+  <si>
+    <t>Art varios ( arena cemento, hidrófugo)</t>
+  </si>
+  <si>
+    <t>Ladrillos</t>
+  </si>
+  <si>
+    <t>Cemento y arena</t>
+  </si>
+  <si>
+    <t>Cierre caja OCT19</t>
+  </si>
+  <si>
     <t>CAJA OCT26</t>
   </si>
   <si>
     <t>Caja OCT26</t>
   </si>
   <si>
-    <t>Una caja</t>
-  </si>
-  <si>
     <t>Caja OCT19</t>
   </si>
   <si>
     <t>Reposición CAJA OCT19</t>
   </si>
   <si>
-    <t>Cierre caja OCT19</t>
-  </si>
-  <si>
     <t>Cierre Caja OCT 19</t>
   </si>
   <si>
-    <t>Caja nuvea</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Un ticket</t>
-  </si>
-  <si>
-    <t>GSP, PICC</t>
-  </si>
-  <si>
-    <t>combustible</t>
+    <t/>
+  </si>
+  <si>
+    <t>Gastos medicos Jose</t>
+  </si>
+  <si>
+    <t>CAMP</t>
+  </si>
+  <si>
+    <t>Peajes</t>
+  </si>
+  <si>
+    <t>peajes</t>
   </si>
   <si>
     <t>b</t>
   </si>
   <si>
+    <t>Flete san Fernando - Artecnia SIN FACTURA</t>
+  </si>
+  <si>
+    <t>Arena y Cemento</t>
+  </si>
+  <si>
+    <t>Volquete - SIN FACTURA</t>
+  </si>
+  <si>
+    <t>Dimmer Cambre - 2da unidad</t>
+  </si>
+  <si>
     <t>Peaje</t>
   </si>
   <si>
-    <t>CAMP</t>
-  </si>
-  <si>
-    <t>peajes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Recambio volquete canton </t>
   </si>
   <si>
-    <t>otros</t>
-  </si>
-  <si>
     <t>Cemento</t>
   </si>
   <si>
@@ -123,34 +183,7 @@
     <t>2 x embudos lluvia duratop xr</t>
   </si>
   <si>
-    <t xml:space="preserve">Combustible </t>
-  </si>
-  <si>
-    <t>LEON</t>
-  </si>
-  <si>
-    <t>Pintura</t>
-  </si>
-  <si>
-    <t>Combustible leonardo</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>Bandejas pintor</t>
-  </si>
-  <si>
-    <t>Flete san Fernando - Artecnia SIN FACTURA</t>
-  </si>
-  <si>
-    <t>Arena y Cemento</t>
-  </si>
-  <si>
-    <t>Volquete - SIN FACTURA</t>
-  </si>
-  <si>
-    <t>Dimmer Cambre - 2da unidad</t>
+    <t>Peajes x 4</t>
   </si>
   <si>
     <t>Lombardi Ferretería - 5 anteojos de protección , masa y cortafierro</t>
@@ -178,6 +211,30 @@
   </si>
   <si>
     <t>AGPA</t>
+  </si>
+  <si>
+    <t>Flete Boris</t>
+  </si>
+  <si>
+    <t>Seguro La Caja MEY 611</t>
+  </si>
+  <si>
+    <t>Bulonera Torcuato - 8 mts de soga</t>
+  </si>
+  <si>
+    <t>Lombardi Ferreteria- Cutter, tizas, lápiz de carpintero</t>
+  </si>
+  <si>
+    <t>Carrefour - bidones de agua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ferretería - bolsas </t>
+  </si>
+  <si>
+    <t>Volcara - volquete</t>
+  </si>
+  <si>
+    <t>Taller Martinez - frenos del auto, mey 611</t>
   </si>
   <si>
     <t>Monto</t>
@@ -650,7 +707,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="8" width="16" customWidth="1"/>
@@ -682,12 +739,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44846</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
       </c>
       <c r="G2">
-        <v>-37500</v>
+        <v>-1600</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -695,114 +767,59 @@
     </row>
     <row r="3" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G3">
-        <v>-56500</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>696969</v>
       </c>
     </row>
     <row r="4" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G4">
-        <v>-696969</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5">
-        <v>-50000</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6">
-        <v>-15500</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="G7">
-        <v>-11500</v>
+        <f>SUM(G2:G5)</f>
       </c>
       <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+        <f>SUM(H2:H5)</f>
+      </c>
+      <c r="I7">
+        <f>SUM(G7,H7)</f>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8">
-        <v>-9400</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>-1723</v>
+      </c>
+    </row>
+    <row r="9" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9">
-        <v>-16000</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12">
-        <f>SUM(G2:G10)</f>
-      </c>
-      <c r="H12">
-        <f>SUM(H2:H10)</f>
-      </c>
-      <c r="I12">
-        <f>SUM(G12,H12)</f>
-      </c>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13">
-        <v>280657</v>
-      </c>
-    </row>
-    <row r="14" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="I15">
-        <f>I14 - I13 - I12</f>
+      <c r="I10">
+        <f>I9 - I8 - I7</f>
       </c>
     </row>
   </sheetData>
@@ -813,7 +830,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I18"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="8" width="16" customWidth="1"/>
@@ -847,63 +864,308 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
-        <v>44846</v>
+        <v>44853</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2">
+        <v>-4206</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44853</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3">
+        <v>-7364</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44853</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>-4207</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44854</v>
+      </c>
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="G2">
-        <v>-1600</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5">
+        <v>-1000</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>9</v>
       </c>
-      <c r="G5">
-        <f>SUM(G2:G3)</f>
-      </c>
-      <c r="H5">
-        <f>SUM(H2:H3)</f>
-      </c>
-      <c r="I5">
-        <f>SUM(G5,H5)</f>
-      </c>
-    </row>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>44855</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
       <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <v>-4000</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>10</v>
       </c>
-      <c r="I6">
-        <v>-1723</v>
-      </c>
-    </row>
-    <row r="7" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>44858</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
       <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>-8800</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>44858</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
       <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>-15000</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>12</v>
       </c>
-      <c r="I8">
-        <f>I7 - I6 - I5</f>
+      <c r="B9" s="1">
+        <v>44859</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9">
+        <v>-2299</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44859</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10">
+        <v>-1100</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44859</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11">
+        <v>-1300</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>11500</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <f>SUM(G2:G13)</f>
+      </c>
+      <c r="H15">
+        <f>SUM(H2:H13)</f>
+      </c>
+      <c r="I15">
+        <f>SUM(G15,H15)</f>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <v>18385</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18">
+        <f>I17 - I16 - I15</f>
       </c>
     </row>
   </sheetData>
@@ -914,7 +1176,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="8" width="16" customWidth="1"/>
@@ -946,221 +1208,94 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44854</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
+    <row r="2" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G2">
-        <v>-100</v>
+        <v>-37500</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44854</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
+    <row r="3" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G3">
-        <v>-100</v>
+        <v>-56500</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44854</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G4">
-        <v>-100</v>
+        <v>-50000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>22</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44854</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G5">
-        <v>-14000</v>
+        <v>-15500</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1">
-        <v>44854</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G6">
-        <v>-5290</v>
+        <v>-9400</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>24</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44854</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7">
-        <v>-5320</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1">
-        <v>44855</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8">
-        <v>-8000</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9">
+        <f>SUM(G2:G7)</f>
+      </c>
+      <c r="H9">
+        <f>SUM(H2:H7)</f>
+      </c>
+      <c r="I9">
+        <f>SUM(G9,H9)</f>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>280657</v>
+      </c>
+    </row>
+    <row r="11" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11">
-        <f>SUM(G2:G9)</f>
-      </c>
-      <c r="H11">
-        <f>SUM(H2:H9)</f>
-      </c>
-      <c r="I11">
-        <f>SUM(G11,H11)</f>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I12">
-        <v>12333</v>
-      </c>
-    </row>
-    <row r="13" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14">
-        <f>I13 - I12 - I11</f>
+        <f>I11 - I10 - I9</f>
       </c>
     </row>
   </sheetData>
@@ -1171,7 +1306,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="8" width="16" customWidth="1"/>
@@ -1205,25 +1340,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>44853</v>
+        <v>44855</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G2">
-        <v>-4206</v>
+        <v>-11458</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1231,25 +1366,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>44853</v>
+        <v>44855</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G3">
-        <v>-7364</v>
+        <v>-8508</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1257,89 +1392,63 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>44853</v>
+        <v>44855</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="G4">
-        <v>-4207</v>
+        <v>-1000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44854</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5">
-        <v>-1000</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <f>SUM(G2:G5)</f>
+      </c>
+      <c r="H7">
+        <f>SUM(H2:H5)</f>
+      </c>
+      <c r="I7">
+        <f>SUM(G7,H7)</f>
       </c>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8">
-        <f>SUM(G2:G6)</f>
-      </c>
-      <c r="H8">
-        <f>SUM(H2:H6)</f>
+        <v>10</v>
       </c>
       <c r="I8">
-        <f>SUM(G8,H8)</f>
-      </c>
-    </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+        <v>19390</v>
+      </c>
+    </row>
+    <row r="9" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9">
-        <v>18512</v>
-      </c>
-    </row>
-    <row r="10" spans="4:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="I11">
-        <f>I10 - I9 - I8</f>
+      <c r="I10">
+        <f>I9 - I8 - I7</f>
       </c>
     </row>
   </sheetData>
@@ -1390,16 +1499,16 @@
         <v>44854</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G2">
         <v>-13500</v>
@@ -1416,16 +1525,16 @@
         <v>44854</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>-2783</v>
@@ -1442,16 +1551,16 @@
         <v>44855</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G4">
         <v>-11000</v>
@@ -1468,16 +1577,16 @@
         <v>44855</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G5">
         <v>-21993</v>
@@ -1529,7 +1638,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I17"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="8" width="16" customWidth="1"/>
@@ -1561,39 +1670,299 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44854</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2">
+        <v>-100</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44854</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3">
+        <v>-100</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44854</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
       <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4">
+        <v>-100</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44854</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5">
+        <v>-14000</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44854</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <v>-5290</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44854</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7">
+        <v>-5320</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44855</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>-8000</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44860</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9">
+        <v>-400</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44858</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10">
+        <v>-320</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44860</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>-5100</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="G4">
-        <f>SUM(G2:G2)</f>
-      </c>
-      <c r="H4">
-        <f>SUM(H2:H2)</f>
-      </c>
-      <c r="I4">
-        <f>SUM(G4,H4)</f>
-      </c>
-    </row>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+      <c r="G14">
+        <f>SUM(G2:G12)</f>
+      </c>
+      <c r="H14">
+        <f>SUM(H2:H12)</f>
+      </c>
+      <c r="I14">
+        <f>SUM(G14,H14)</f>
+      </c>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
         <v>10</v>
       </c>
-      <c r="I5">
-        <v>19390</v>
-      </c>
-    </row>
-    <row r="6" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+      <c r="I15">
+        <v>12333</v>
+      </c>
+    </row>
+    <row r="16" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
         <v>12</v>
       </c>
-      <c r="I7">
-        <f>I6 - I5 - I4</f>
+      <c r="I17">
+        <f>I16 - I15 - I14</f>
       </c>
     </row>
   </sheetData>
@@ -1604,7 +1973,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I21"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="8" width="16" customWidth="1"/>
@@ -1644,16 +2013,16 @@
         <v>44854</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G2">
         <v>-7780</v>
@@ -1670,16 +2039,16 @@
         <v>44854</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>-2370</v>
@@ -1696,16 +2065,16 @@
         <v>44854</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="G4">
         <v>-600</v>
@@ -1722,16 +2091,16 @@
         <v>44854</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G5">
         <v>-4254</v>
@@ -1748,16 +2117,16 @@
         <v>44855</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G6">
         <v>-9500</v>
@@ -1774,16 +2143,16 @@
         <v>44855</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G7">
         <v>-10000</v>
@@ -1792,39 +2161,247 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44856</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>-6000</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44856</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9">
+        <v>-11132</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44858</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
       <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10">
+        <v>-746</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44858</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11">
+        <v>-1740</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44859</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12">
+        <v>-706</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44858</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13">
+        <v>-1980</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44855</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14">
+        <v>-9500</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44847</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15">
+        <v>-19000</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
         <v>9</v>
       </c>
-      <c r="G10">
-        <f>SUM(G2:G8)</f>
-      </c>
-      <c r="H10">
-        <f>SUM(H2:H8)</f>
-      </c>
-      <c r="I10">
-        <f>SUM(G10,H10)</f>
-      </c>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+      <c r="G18">
+        <f>SUM(G2:G16)</f>
+      </c>
+      <c r="H18">
+        <f>SUM(H2:H16)</f>
+      </c>
+      <c r="I18">
+        <f>SUM(G18,H18)</f>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
         <v>10</v>
       </c>
-      <c r="I11">
+      <c r="I19">
         <v>43431</v>
       </c>
     </row>
-    <row r="12" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
         <v>12</v>
       </c>
-      <c r="I13">
-        <f>I12 - I11 - I10</f>
+      <c r="I21">
+        <f>I20 - I19 - I18</f>
       </c>
     </row>
   </sheetData>
@@ -1835,7 +2412,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="16" customWidth="1"/>
@@ -1846,36 +2423,36 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B2">
-        <v>24504</v>
+        <v>57430</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B3">
-        <v>32910</v>
+        <v>47238</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>66053</v>
+        <v>85053</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B5">
         <v>1600</v>
@@ -1883,7 +2460,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="B6">
         <v>1600</v>
@@ -1891,10 +2468,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B7">
-        <v>10000</v>
+        <v>27878</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>13499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>